<commit_message>
reso il collegamento alla pagina un URI
</commit_message>
<xml_diff>
--- a/data/mapping_doc_link.xlsx
+++ b/data/mapping_doc_link.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP 149889\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP 149889\PycharmProjects\EVA-KG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85A490F-E86B-400B-A6FD-069888DD2541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137A3979-5577-4C19-A229-4F9691F28165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,21 +464,12 @@
     <t>LinkAlt</t>
   </si>
   <si>
-    <t>CASE OF S.Z. v. BULGARIA</t>
-  </si>
-  <si>
     <t>https://hudoc.echr.coe.int/#{%22itemid%22:[%22001-152850%22]}</t>
   </si>
   <si>
-    <t>CASE OF TALPIS v. ITALY</t>
-  </si>
-  <si>
     <t>https://hudoc.echr.coe.int/#{%22itemid%22:[%22001-171994%22]}</t>
   </si>
   <si>
-    <t>CASE OF BUTURUGĂ v. ROMANIA</t>
-  </si>
-  <si>
     <t>https://hudoc.echr.coe.int/#{%22itemid%22:[%22001-201342%22]}</t>
   </si>
   <si>
@@ -486,6 +477,15 @@
   </si>
   <si>
     <t>https://hudoc.echr.coe.int/#{%22itemid%22:[%22001-209373%22]}</t>
+  </si>
+  <si>
+    <t>CASE OF TALPIS v. ITALY</t>
+  </si>
+  <si>
+    <t>CASE OF S.Z. v. BULGARIA</t>
+  </si>
+  <si>
+    <t>CASE OF BUTURUGĂ v. ROMANIA</t>
   </si>
 </sst>
 </file>
@@ -536,12 +536,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -621,6 +620,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DD5A9B4-6FF9-45F1-8C45-ACB5CE9862F2}" name="Tabella3" displayName="Tabella3" ref="A1:C74" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A1:C74" xr:uid="{4DD5A9B4-6FF9-45F1-8C45-ACB5CE9862F2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C74">
+    <sortCondition ref="A1:A74"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B24E2B5D-1CA3-4E78-A4AE-5E86881EFD53}" name="Titolo" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{BE28A509-98B6-4F26-8E60-ADCF5C484F7D}" name="Link" dataDxfId="1" dataCellStyle="Collegamento ipertestuale"/>
@@ -897,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,722 +1082,722 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-93955"]}</v>
+        <v>https://hudoc.echr.coe.int/#{"itemid":["001-209373"]}</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-119968"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-93955"]}</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-211592"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-119968"]}</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"dmdocnumber":["877609"],"itemid":["001-101945"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-211592"]}</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-110904"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"dmdocnumber":["877609"],"itemid":["001-101945"]}</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-154152"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-110904"]}</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-167118"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-154152"]}</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-170388"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-167118"]}</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-196897"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-170388"]}</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-219067"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-196897"]}</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-86255"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-219067"]}</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"dmdocnumber":["907057"],"itemid":["001-110452"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-86255"]}</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-80696"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"dmdocnumber":["907057"],"itemid":["001-110452"]}</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng/#{"itemid":["001-210463"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-80696"]}</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-203931"]}</v>
+        <v>https://hudoc.echr.coe.int/eng/#{"itemid":["001-210463"]}</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-112576"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-203931"]}</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C31" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-150318"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-112576"]}</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-61521"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-150318"]}</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-220867"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-61521"]}</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C34" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-84670"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-220867"]}</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-122375"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-84670"]}</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-202554"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-122375"]}</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-99992"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-202554"]}</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-150310"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-99992"]}</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-193069"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-150310"]}</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-140235"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-193069"]}</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-92945"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-140235"]}</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C42" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-114098"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-92945"]}</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C43" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"dmdocnumber":["899269"],"itemid":["001-108781"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-114098"]}</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C44" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-96549"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"dmdocnumber":["899269"],"itemid":["001-108781"]}</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C45" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-144137"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-96549"]}</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C46" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-203503"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-144137"]}</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C47" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/fre#{"itemid":["001-207360"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-203503"]}</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C48" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-91608"]}</v>
+        <v>https://hudoc.echr.coe.int/fre#{"itemid":["001-207360"]}</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C49" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-140240"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-91608"]}</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C50" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-203825"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-140240"]}</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C51" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-210854"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-203825"]}</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C52" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-213869"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-210854"]}</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C53" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-117636"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-213869"]}</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C54" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-194321"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-117636"]}</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C55" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-211794"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-194321"]}</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C56" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-140030"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-211794"]}</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C57" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-57603"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-140030"]}</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C58" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-216360"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-57603"]}</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C59" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-154728"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-216360"]}</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C60" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-109557"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-154728"]}</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C61" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-61247"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-109557"]}</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C62" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-175142"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-61247"]}</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C63" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-79864"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-175142"]}</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="C64" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-138514"]}</v>
+        <v>https://hudoc.echr.coe.int/#{"itemid":["001-201342"]}</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C65" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-127061"]}</v>
+        <v>https://hudoc.echr.coe.int/#{"itemid":["001-152850"]}</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C66" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-114397"]}</v>
+        <v>https://hudoc.echr.coe.int/#{"itemid":["001-171994"]}</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C67" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-105081"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-79864"]}</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C68" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-113956"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-138514"]}</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C69" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-106527"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-127061"]}</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C70" s="1" t="str">
         <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-150572"]}</v>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-114397"]}</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C71" s="4" t="str">
-        <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/#{"itemid":["001-152850"]}</v>
+        <v>131</v>
+      </c>
+      <c r="C71" s="1" t="str">
+        <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-105081"]}</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C72" s="4" t="str">
-        <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/#{"itemid":["001-171994"]}</v>
+        <v>133</v>
+      </c>
+      <c r="C72" s="1" t="str">
+        <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-113956"]}</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C73" s="4" t="str">
-        <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/#{"itemid":["001-201342"]}</v>
+        <v>135</v>
+      </c>
+      <c r="C73" s="1" t="str">
+        <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-106527"]}</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C74" s="4" t="str">
-        <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
-        <v>https://hudoc.echr.coe.int/#{"itemid":["001-209373"]}</v>
+        <v>137</v>
+      </c>
+      <c r="C74" s="1" t="str">
+        <f>SUBSTITUTE(Tabella3[[#This Row],[Link]], "%22", """")</f>
+        <v>https://hudoc.echr.coe.int/eng#{"itemid":["001-150572"]}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>